<commit_message>
Commit progress on starfield
</commit_message>
<xml_diff>
--- a/Invaders/Randomnumbers.xlsx
+++ b/Invaders/Randomnumbers.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uersu\Documents\GitData\voidanniversary\Invaders\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8535C3EB-EB4C-4A11-906D-542E3CF0E918}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9996E65E-8802-417E-ACC1-A40E7A9512C0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20760" windowHeight="13320" xr2:uid="{5B282EBC-E1FB-4CFE-92EC-3ABF1BA2B9BE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{5B282EBC-E1FB-4CFE-92EC-3ABF1BA2B9BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
-    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
+    <sheet name="Xtable" sheetId="2" r:id="rId2"/>
+    <sheet name="Tabelle2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,19 +27,22 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
   <si>
     <t>Zufallszahl</t>
   </si>
   <si>
     <t>Assembler</t>
   </si>
+  <si>
+    <t>Zahl</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -46,19 +50,73 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor theme="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -67,13 +125,55 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="6">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="1"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -97,11 +197,37 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FD13CB3B-AC0E-4A23-BCB6-EC36AD1D4C8A}" name="Tabelle1" displayName="Tabelle1" ref="A1:B101" totalsRowShown="0">
   <autoFilter ref="A1:B101" xr:uid="{4F6840FD-F35F-431E-85ED-D973CB27593B}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{D37C4E92-5377-42F2-8281-936C5A9011EA}" name="Zufallszahl" dataDxfId="1">
+    <tableColumn id="1" xr3:uid="{D37C4E92-5377-42F2-8281-936C5A9011EA}" name="Zufallszahl" dataDxfId="5">
       <calculatedColumnFormula>INT(1+RAND()*3)*IF(RAND()&gt;0.5,1,-1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{413D3B5B-E546-4B71-AF67-9B7F88CA5091}" name="Assembler" dataDxfId="0">
+    <tableColumn id="2" xr3:uid="{413D3B5B-E546-4B71-AF67-9B7F88CA5091}" name="Assembler" dataDxfId="4">
       <calculatedColumnFormula>"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{65D73A58-C1FD-4D9C-AA78-E5023721494C}" name="Tabelle2" displayName="Tabelle2" ref="A1:B101" totalsRowShown="0">
+  <autoFilter ref="A1:B101" xr:uid="{05F44B28-C440-458D-A5A3-EC3C29E0377B}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{00F2F601-E68B-4BEE-A52D-1AD593E72D44}" name="Zahl"/>
+    <tableColumn id="2" xr3:uid="{57C4C8A9-0214-451A-8A1A-2A7AB327381D}" name="Assembler" dataDxfId="3">
+      <calculatedColumnFormula>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{162A8026-03F6-43AF-91D5-F9E735F860C8}" name="Tabelle3" displayName="Tabelle3" ref="A1:B101" totalsRowShown="0" headerRowDxfId="1" tableBorderDxfId="2">
+  <autoFilter ref="A1:B101" xr:uid="{32C7B4C3-C1BA-4CE3-ADA2-0277496CD58E}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{FB6A680A-E412-4CE9-995A-C77644EA0452}" name="Zahl"/>
+    <tableColumn id="2" xr3:uid="{4404A6C7-311F-41B3-AB7F-8CC989516026}" name="Assembler" dataDxfId="0">
+      <calculatedColumnFormula>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -407,8 +533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E9C8814-83B2-440E-A369-49B1CBED393C}">
   <dimension ref="A1:B101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,11 +553,11 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <f t="shared" ref="A2:A33" ca="1" si="0">INT(1+RAND()*3)*IF(RAND()&gt;0.5,1,-1)</f>
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="B2" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -1</v>
+        <v>dc.w -3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -447,41 +573,41 @@
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 1</v>
+        <v>dc.w 2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" ca="1" si="0"/>
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="B5" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -2</v>
+        <v>dc.w -1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" ca="1" si="0"/>
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="B6" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -2</v>
+        <v>dc.w -1</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B7" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 1</v>
+        <v>dc.w 2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -497,141 +623,141 @@
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B9" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 1</v>
+        <v>dc.w 2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" ca="1" si="0"/>
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="B10" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -2</v>
+        <v>dc.w 2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B11" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 3</v>
+        <v>dc.w 2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" ca="1" si="0"/>
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="B12" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -3</v>
+        <v>dc.w -1</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" ca="1" si="0"/>
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="B13" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -1</v>
+        <v>dc.w 3</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>-3</v>
       </c>
       <c r="B14" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 3</v>
+        <v>dc.w -3</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B15" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 1</v>
+        <v>dc.w 3</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" ca="1" si="0"/>
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="B16" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -2</v>
+        <v>dc.w -1</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="B17" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 3</v>
+        <v>dc.w -1</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="B18" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 2</v>
+        <v>dc.w -3</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" ca="1" si="0"/>
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="B19" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -3</v>
+        <v>dc.w -1</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>-3</v>
       </c>
       <c r="B20" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 3</v>
+        <v>dc.w -3</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B21" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 3</v>
+        <v>dc.w 2</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" ca="1" si="0"/>
-        <v>-2</v>
+        <v>3</v>
       </c>
       <c r="B22" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -2</v>
+        <v>dc.w 3</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -647,61 +773,61 @@
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" ca="1" si="0"/>
-        <v>-3</v>
+        <v>2</v>
       </c>
       <c r="B24" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -3</v>
+        <v>dc.w 2</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B25" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 1</v>
+        <v>dc.w -1</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" ca="1" si="0"/>
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="B26" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -2</v>
+        <v>dc.w -1</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" ca="1" si="0"/>
-        <v>-2</v>
+        <v>3</v>
       </c>
       <c r="B27" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -2</v>
+        <v>dc.w 3</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="B28" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 2</v>
+        <v>dc.w -3</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="B29" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 2</v>
+        <v>dc.w -2</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -717,31 +843,31 @@
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" ca="1" si="0"/>
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="B31" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -1</v>
+        <v>dc.w -3</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B32" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 1</v>
+        <v>dc.w -1</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" ca="1" si="0"/>
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="B33" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -1</v>
+        <v>dc.w 3</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -757,211 +883,211 @@
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" ca="1" si="1"/>
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="B35" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -2</v>
+        <v>dc.w -3</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
         <f t="shared" ca="1" si="1"/>
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="B36" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -2</v>
+        <v>dc.w -1</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
         <f t="shared" ca="1" si="1"/>
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="B37" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -1</v>
+        <v>dc.w 3</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>-3</v>
       </c>
       <c r="B38" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 3</v>
+        <v>dc.w -3</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>-3</v>
       </c>
       <c r="B39" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 3</v>
+        <v>dc.w -3</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>-3</v>
       </c>
       <c r="B40" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 1</v>
+        <v>dc.w -3</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B41" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 1</v>
+        <v>dc.w 2</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B42" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 1</v>
+        <v>dc.w 2</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="B43" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 2</v>
+        <v>dc.w -2</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44">
         <f t="shared" ca="1" si="1"/>
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="B44" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -1</v>
+        <v>dc.w -3</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="B45" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 2</v>
+        <v>dc.w -3</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B46" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 3</v>
+        <v>dc.w 2</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47">
         <f t="shared" ca="1" si="1"/>
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="B47" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -3</v>
+        <v>dc.w -1</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B48" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 1</v>
+        <v>dc.w 2</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49">
         <f t="shared" ca="1" si="1"/>
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="B49" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -1</v>
+        <v>dc.w 2</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50">
         <f t="shared" ca="1" si="1"/>
-        <v>-2</v>
+        <v>1</v>
       </c>
       <c r="B50" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -2</v>
+        <v>dc.w 1</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="B51" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 3</v>
+        <v>dc.w -1</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52">
         <f t="shared" ca="1" si="1"/>
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="B52" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -1</v>
+        <v>dc.w 2</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>-3</v>
       </c>
       <c r="B53" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 1</v>
+        <v>dc.w -3</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54">
         <f t="shared" ca="1" si="1"/>
-        <v>-2</v>
+        <v>1</v>
       </c>
       <c r="B54" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -2</v>
+        <v>dc.w 1</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="B55" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 2</v>
+        <v>dc.w -2</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -977,61 +1103,61 @@
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B57" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 2</v>
+        <v>dc.w 1</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B58" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 1</v>
+        <v>dc.w 3</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59">
         <f t="shared" ca="1" si="1"/>
-        <v>-3</v>
+        <v>3</v>
       </c>
       <c r="B59" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -3</v>
+        <v>dc.w 3</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B60" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 3</v>
+        <v>dc.w 2</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B61" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 3</v>
+        <v>dc.w 2</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62">
         <f t="shared" ca="1" si="1"/>
-        <v>-3</v>
+        <v>1</v>
       </c>
       <c r="B62" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -3</v>
+        <v>dc.w 1</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -1047,91 +1173,91 @@
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64">
         <f t="shared" ca="1" si="1"/>
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="B64" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -3</v>
+        <v>dc.w -1</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65">
         <f t="shared" ca="1" si="1"/>
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="B65" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -1</v>
+        <v>dc.w 3</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66">
         <f t="shared" ref="A66:A101" ca="1" si="2">INT(1+RAND()*3)*IF(RAND()&gt;0.5,1,-1)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B66" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 2</v>
+        <v>dc.w 3</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>-3</v>
       </c>
       <c r="B67" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 3</v>
+        <v>dc.w -3</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>-3</v>
       </c>
       <c r="B68" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 3</v>
+        <v>dc.w -3</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B69" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 2</v>
+        <v>dc.w 1</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B70" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 2</v>
+        <v>dc.w 3</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B71" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 2</v>
+        <v>dc.w 3</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B72" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 1</v>
+        <v>dc.w 3</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -1147,21 +1273,21 @@
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="B74" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 2</v>
+        <v>dc.w -2</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="B75" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 2</v>
+        <v>dc.w -2</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -1177,41 +1303,41 @@
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77">
         <f t="shared" ca="1" si="2"/>
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="B77" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -1</v>
+        <v>dc.w 2</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78">
         <f t="shared" ca="1" si="2"/>
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="B78" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -2</v>
+        <v>dc.w -3</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79">
         <f t="shared" ca="1" si="2"/>
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="B79" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -1</v>
+        <v>dc.w -3</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B80" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 1</v>
+        <v>dc.w 3</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
@@ -1237,31 +1363,31 @@
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="B83" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 3</v>
+        <v>dc.w -1</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B84" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 1</v>
+        <v>dc.w -1</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>-2</v>
       </c>
       <c r="B85" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 3</v>
+        <v>dc.w -2</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
@@ -1277,71 +1403,71 @@
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87">
         <f t="shared" ca="1" si="2"/>
-        <v>-3</v>
+        <v>2</v>
       </c>
       <c r="B87" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -3</v>
+        <v>dc.w 2</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88">
         <f t="shared" ca="1" si="2"/>
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="B88" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -2</v>
+        <v>dc.w 2</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B89" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 1</v>
+        <v>dc.w 3</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90">
         <f t="shared" ca="1" si="2"/>
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="B90" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -1</v>
+        <v>dc.w 3</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>-3</v>
       </c>
       <c r="B91" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 1</v>
+        <v>dc.w -3</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92">
         <f t="shared" ca="1" si="2"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B92" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -1</v>
+        <v>dc.w 1</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B93" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 2</v>
+        <v>dc.w 1</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
@@ -1357,71 +1483,71 @@
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>-2</v>
       </c>
       <c r="B95" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 3</v>
+        <v>dc.w -2</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B96" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 3</v>
+        <v>dc.w 2</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>-2</v>
       </c>
       <c r="B97" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 3</v>
+        <v>dc.w -2</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="B98" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 2</v>
+        <v>dc.w -2</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B99" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 1</v>
+        <v>dc.w -1</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100">
         <f t="shared" ca="1" si="2"/>
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="B100" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -3</v>
+        <v>dc.w -2</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="B101" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 2</v>
+        <v>dc.w -1</v>
       </c>
     </row>
   </sheetData>
@@ -1434,12 +1560,1867 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E59E07D8-3039-4DAB-963A-47C134361A80}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B101"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="B101" sqref="B101"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>-1</v>
+      </c>
+      <c r="B2" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>-2</v>
+      </c>
+      <c r="B3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>-3</v>
+      </c>
+      <c r="B4" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>-4</v>
+      </c>
+      <c r="B5" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>-5</v>
+      </c>
+      <c r="B6" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>4</v>
+      </c>
+      <c r="B10" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>-1</v>
+      </c>
+      <c r="B12" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>-2</v>
+      </c>
+      <c r="B13" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>-3</v>
+      </c>
+      <c r="B14" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>-4</v>
+      </c>
+      <c r="B15" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>-5</v>
+      </c>
+      <c r="B16" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>3</v>
+      </c>
+      <c r="B19" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>4</v>
+      </c>
+      <c r="B20" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>5</v>
+      </c>
+      <c r="B21" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>-1</v>
+      </c>
+      <c r="B22" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>-2</v>
+      </c>
+      <c r="B23" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>-3</v>
+      </c>
+      <c r="B24" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>-4</v>
+      </c>
+      <c r="B25" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>-5</v>
+      </c>
+      <c r="B26" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>2</v>
+      </c>
+      <c r="B28" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>3</v>
+      </c>
+      <c r="B29" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>4</v>
+      </c>
+      <c r="B30" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>5</v>
+      </c>
+      <c r="B31" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>-1</v>
+      </c>
+      <c r="B32" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>-2</v>
+      </c>
+      <c r="B33" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>-3</v>
+      </c>
+      <c r="B34" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>-4</v>
+      </c>
+      <c r="B35" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>-5</v>
+      </c>
+      <c r="B36" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>1</v>
+      </c>
+      <c r="B37" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>2</v>
+      </c>
+      <c r="B38" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>3</v>
+      </c>
+      <c r="B39" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>4</v>
+      </c>
+      <c r="B40" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>5</v>
+      </c>
+      <c r="B41" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>-1</v>
+      </c>
+      <c r="B42" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>-2</v>
+      </c>
+      <c r="B43" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>-3</v>
+      </c>
+      <c r="B44" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>-4</v>
+      </c>
+      <c r="B45" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>-5</v>
+      </c>
+      <c r="B46" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>1</v>
+      </c>
+      <c r="B47" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>2</v>
+      </c>
+      <c r="B48" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>3</v>
+      </c>
+      <c r="B49" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>4</v>
+      </c>
+      <c r="B50" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>5</v>
+      </c>
+      <c r="B51" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>-1</v>
+      </c>
+      <c r="B52" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>-2</v>
+      </c>
+      <c r="B53" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>-3</v>
+      </c>
+      <c r="B54" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>-4</v>
+      </c>
+      <c r="B55" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>-5</v>
+      </c>
+      <c r="B56" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>1</v>
+      </c>
+      <c r="B57" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>2</v>
+      </c>
+      <c r="B58" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>3</v>
+      </c>
+      <c r="B59" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>4</v>
+      </c>
+      <c r="B60" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>5</v>
+      </c>
+      <c r="B61" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>-1</v>
+      </c>
+      <c r="B62" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>-2</v>
+      </c>
+      <c r="B63" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>-3</v>
+      </c>
+      <c r="B64" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>-4</v>
+      </c>
+      <c r="B65" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>-5</v>
+      </c>
+      <c r="B66" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>1</v>
+      </c>
+      <c r="B67" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>2</v>
+      </c>
+      <c r="B68" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>3</v>
+      </c>
+      <c r="B69" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>4</v>
+      </c>
+      <c r="B70" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>5</v>
+      </c>
+      <c r="B71" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>-1</v>
+      </c>
+      <c r="B72" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>-2</v>
+      </c>
+      <c r="B73" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>-3</v>
+      </c>
+      <c r="B74" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>-4</v>
+      </c>
+      <c r="B75" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -4</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>-5</v>
+      </c>
+      <c r="B76" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>1</v>
+      </c>
+      <c r="B77" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>2</v>
+      </c>
+      <c r="B78" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>3</v>
+      </c>
+      <c r="B79" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>4</v>
+      </c>
+      <c r="B80" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>5</v>
+      </c>
+      <c r="B81" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>-1</v>
+      </c>
+      <c r="B82" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>-2</v>
+      </c>
+      <c r="B83" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>-3</v>
+      </c>
+      <c r="B84" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>-4</v>
+      </c>
+      <c r="B85" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -4</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>-5</v>
+      </c>
+      <c r="B86" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>1</v>
+      </c>
+      <c r="B87" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>2</v>
+      </c>
+      <c r="B88" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>3</v>
+      </c>
+      <c r="B89" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>4</v>
+      </c>
+      <c r="B90" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 4</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>5</v>
+      </c>
+      <c r="B91" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>-1</v>
+      </c>
+      <c r="B92" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>-2</v>
+      </c>
+      <c r="B93" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>-3</v>
+      </c>
+      <c r="B94" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>-4</v>
+      </c>
+      <c r="B95" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -4</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>-5</v>
+      </c>
+      <c r="B96" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>1</v>
+      </c>
+      <c r="B97" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>2</v>
+      </c>
+      <c r="B98" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>3</v>
+      </c>
+      <c r="B99" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 3</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>4</v>
+      </c>
+      <c r="B100" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 4</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>5</v>
+      </c>
+      <c r="B101" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C888866-0535-4EEA-B92A-DFAC3598319B}">
+  <dimension ref="A1:B104"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="B105" sqref="B105"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>-5</v>
+      </c>
+      <c r="B2" s="2" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w -5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>-5</v>
+      </c>
+      <c r="B3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w -5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>-5</v>
+      </c>
+      <c r="B4" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w -5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>-5</v>
+      </c>
+      <c r="B5" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w -5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>-5</v>
+      </c>
+      <c r="B6" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w -5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>-5</v>
+      </c>
+      <c r="B7" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w -5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>-5</v>
+      </c>
+      <c r="B8" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w -5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>-5</v>
+      </c>
+      <c r="B9" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w -5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>-5</v>
+      </c>
+      <c r="B10" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w -5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>-5</v>
+      </c>
+      <c r="B11" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w -5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>-4</v>
+      </c>
+      <c r="B12" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w -4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>-4</v>
+      </c>
+      <c r="B13" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w -4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>-4</v>
+      </c>
+      <c r="B14" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w -4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>-4</v>
+      </c>
+      <c r="B15" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w -4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>-4</v>
+      </c>
+      <c r="B16" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w -4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>-4</v>
+      </c>
+      <c r="B17" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w -4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>-4</v>
+      </c>
+      <c r="B18" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w -4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>-4</v>
+      </c>
+      <c r="B19" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w -4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>-4</v>
+      </c>
+      <c r="B20" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w -4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>-4</v>
+      </c>
+      <c r="B21" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w -4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>-3</v>
+      </c>
+      <c r="B22" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w -3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>-3</v>
+      </c>
+      <c r="B23" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w -3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>-3</v>
+      </c>
+      <c r="B24" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w -3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>-3</v>
+      </c>
+      <c r="B25" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w -3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>-3</v>
+      </c>
+      <c r="B26" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w -3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>-3</v>
+      </c>
+      <c r="B27" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w -3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>-3</v>
+      </c>
+      <c r="B28" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w -3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>-3</v>
+      </c>
+      <c r="B29" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w -3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>-3</v>
+      </c>
+      <c r="B30" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w -3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>-3</v>
+      </c>
+      <c r="B31" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w -3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>-2</v>
+      </c>
+      <c r="B32" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w -2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>-2</v>
+      </c>
+      <c r="B33" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w -2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>-2</v>
+      </c>
+      <c r="B34" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w -2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>-2</v>
+      </c>
+      <c r="B35" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w -2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>-2</v>
+      </c>
+      <c r="B36" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w -2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>-2</v>
+      </c>
+      <c r="B37" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w -2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>-2</v>
+      </c>
+      <c r="B38" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w -2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>-2</v>
+      </c>
+      <c r="B39" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w -2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>-2</v>
+      </c>
+      <c r="B40" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w -2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>-2</v>
+      </c>
+      <c r="B41" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w -2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>-1</v>
+      </c>
+      <c r="B42" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w -1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>-1</v>
+      </c>
+      <c r="B43" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w -1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>-1</v>
+      </c>
+      <c r="B44" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w -1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>-1</v>
+      </c>
+      <c r="B45" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w -1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>-1</v>
+      </c>
+      <c r="B46" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w -1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>-1</v>
+      </c>
+      <c r="B47" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w -1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>-1</v>
+      </c>
+      <c r="B48" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w -1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>-1</v>
+      </c>
+      <c r="B49" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w -1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>-1</v>
+      </c>
+      <c r="B50" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w -1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>-1</v>
+      </c>
+      <c r="B51" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w -1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>1</v>
+      </c>
+      <c r="B52" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>1</v>
+      </c>
+      <c r="B53" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>1</v>
+      </c>
+      <c r="B54" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>1</v>
+      </c>
+      <c r="B55" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>1</v>
+      </c>
+      <c r="B56" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>1</v>
+      </c>
+      <c r="B57" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>1</v>
+      </c>
+      <c r="B58" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>1</v>
+      </c>
+      <c r="B59" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>1</v>
+      </c>
+      <c r="B60" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>1</v>
+      </c>
+      <c r="B61" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>2</v>
+      </c>
+      <c r="B62" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>2</v>
+      </c>
+      <c r="B63" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>2</v>
+      </c>
+      <c r="B64" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>2</v>
+      </c>
+      <c r="B65" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>2</v>
+      </c>
+      <c r="B66" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>2</v>
+      </c>
+      <c r="B67" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>2</v>
+      </c>
+      <c r="B68" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>2</v>
+      </c>
+      <c r="B69" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>2</v>
+      </c>
+      <c r="B70" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>2</v>
+      </c>
+      <c r="B71" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>3</v>
+      </c>
+      <c r="B72" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>3</v>
+      </c>
+      <c r="B73" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>3</v>
+      </c>
+      <c r="B74" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>3</v>
+      </c>
+      <c r="B75" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>3</v>
+      </c>
+      <c r="B76" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>3</v>
+      </c>
+      <c r="B77" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>3</v>
+      </c>
+      <c r="B78" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>3</v>
+      </c>
+      <c r="B79" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>3</v>
+      </c>
+      <c r="B80" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>3</v>
+      </c>
+      <c r="B81" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>4</v>
+      </c>
+      <c r="B82" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 4</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>4</v>
+      </c>
+      <c r="B83" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>4</v>
+      </c>
+      <c r="B84" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 4</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>4</v>
+      </c>
+      <c r="B85" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 4</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>4</v>
+      </c>
+      <c r="B86" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>4</v>
+      </c>
+      <c r="B87" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 4</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>4</v>
+      </c>
+      <c r="B88" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>4</v>
+      </c>
+      <c r="B89" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 4</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>4</v>
+      </c>
+      <c r="B90" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 4</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>4</v>
+      </c>
+      <c r="B91" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>5</v>
+      </c>
+      <c r="B92" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>5</v>
+      </c>
+      <c r="B93" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>5</v>
+      </c>
+      <c r="B94" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 5</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>5</v>
+      </c>
+      <c r="B95" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 5</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>5</v>
+      </c>
+      <c r="B96" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>5</v>
+      </c>
+      <c r="B97" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>5</v>
+      </c>
+      <c r="B98" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 5</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>5</v>
+      </c>
+      <c r="B99" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 5</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>5</v>
+      </c>
+      <c r="B100" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>5</v>
+      </c>
+      <c r="B101" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 5</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B102" s="3"/>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B103" s="3"/>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B104" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Something that remotely resembles a starfield
</commit_message>
<xml_diff>
--- a/Invaders/Randomnumbers.xlsx
+++ b/Invaders/Randomnumbers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uersu\Documents\GitData\voidanniversary\Invaders\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9996E65E-8802-417E-ACC1-A40E7A9512C0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A10AD5B6-83DA-4CD9-9505-AC77A216F66A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{5B282EBC-E1FB-4CFE-92EC-3ABF1BA2B9BE}"/>
   </bookViews>
@@ -141,6 +141,13 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -163,13 +170,6 @@
           <bgColor theme="1"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -209,8 +209,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{65D73A58-C1FD-4D9C-AA78-E5023721494C}" name="Tabelle2" displayName="Tabelle2" ref="A1:B101" totalsRowShown="0">
-  <autoFilter ref="A1:B101" xr:uid="{05F44B28-C440-458D-A5A3-EC3C29E0377B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{65D73A58-C1FD-4D9C-AA78-E5023721494C}" name="Tabelle2" displayName="Tabelle2" ref="A1:B197" totalsRowShown="0">
+  <autoFilter ref="A1:B197" xr:uid="{05F44B28-C440-458D-A5A3-EC3C29E0377B}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00F2F601-E68B-4BEE-A52D-1AD593E72D44}" name="Zahl"/>
     <tableColumn id="2" xr3:uid="{57C4C8A9-0214-451A-8A1A-2A7AB327381D}" name="Assembler" dataDxfId="3">
@@ -222,8 +222,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{162A8026-03F6-43AF-91D5-F9E735F860C8}" name="Tabelle3" displayName="Tabelle3" ref="A1:B101" totalsRowShown="0" headerRowDxfId="1" tableBorderDxfId="2">
-  <autoFilter ref="A1:B101" xr:uid="{32C7B4C3-C1BA-4CE3-ADA2-0277496CD58E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{162A8026-03F6-43AF-91D5-F9E735F860C8}" name="Tabelle3" displayName="Tabelle3" ref="A1:B197" totalsRowShown="0" headerRowDxfId="2" tableBorderDxfId="1">
+  <autoFilter ref="A1:B197" xr:uid="{32C7B4C3-C1BA-4CE3-ADA2-0277496CD58E}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{FB6A680A-E412-4CE9-995A-C77644EA0452}" name="Zahl"/>
     <tableColumn id="2" xr3:uid="{4404A6C7-311F-41B3-AB7F-8CC989516026}" name="Assembler" dataDxfId="0">
@@ -553,91 +553,91 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <f t="shared" ref="A2:A33" ca="1" si="0">INT(1+RAND()*3)*IF(RAND()&gt;0.5,1,-1)</f>
-        <v>-3</v>
+        <v>1</v>
       </c>
       <c r="B2" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -3</v>
+        <v>dc.w 1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" ca="1" si="0"/>
-        <v>-2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -2</v>
+        <v>dc.w 1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="B4" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 2</v>
+        <v>dc.w -3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" ca="1" si="0"/>
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="B5" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -1</v>
+        <v>dc.w 3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" ca="1" si="0"/>
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="B6" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -1</v>
+        <v>dc.w -2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="B7" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 2</v>
+        <v>dc.w -1</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B8" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 1</v>
+        <v>dc.w -1</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="B9" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 2</v>
+        <v>dc.w -3</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B10" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 2</v>
+        <v>dc.w 1</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -663,81 +663,81 @@
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B13" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 3</v>
+        <v>dc.w 2</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" ca="1" si="0"/>
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="B14" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -3</v>
+        <v>dc.w -1</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B15" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 3</v>
+        <v>dc.w 1</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" ca="1" si="0"/>
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="B16" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -1</v>
+        <v>dc.w -3</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" ca="1" si="0"/>
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="B17" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -1</v>
+        <v>dc.w 2</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" ca="1" si="0"/>
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="B18" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -3</v>
+        <v>dc.w -2</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" ca="1" si="0"/>
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="B19" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -1</v>
+        <v>dc.w -2</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" ca="1" si="0"/>
-        <v>-3</v>
+        <v>2</v>
       </c>
       <c r="B20" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -3</v>
+        <v>dc.w 2</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -763,31 +763,31 @@
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" ca="1" si="0"/>
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="B23" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -2</v>
+        <v>dc.w -3</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B24" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 2</v>
+        <v>dc.w 3</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" ca="1" si="0"/>
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="B25" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -1</v>
+        <v>dc.w 2</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -803,51 +803,51 @@
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>-2</v>
       </c>
       <c r="B27" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 3</v>
+        <v>dc.w -2</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" ca="1" si="0"/>
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="B28" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -3</v>
+        <v>dc.w -2</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" ca="1" si="0"/>
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="B29" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -2</v>
+        <v>dc.w -3</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" ca="1" si="0"/>
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="B30" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -3</v>
+        <v>dc.w -2</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" ca="1" si="0"/>
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="B31" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -3</v>
+        <v>dc.w -1</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -863,31 +863,31 @@
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>-2</v>
       </c>
       <c r="B33" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 3</v>
+        <v>dc.w -2</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" ref="A34:A65" ca="1" si="1">INT(1+RAND()*3)*IF(RAND()&gt;0.5,1,-1)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B34" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 2</v>
+        <v>dc.w 1</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" ca="1" si="1"/>
-        <v>-3</v>
+        <v>1</v>
       </c>
       <c r="B35" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -3</v>
+        <v>dc.w 1</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -903,31 +903,31 @@
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="B37" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 3</v>
+        <v>dc.w -1</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" ca="1" si="1"/>
-        <v>-3</v>
+        <v>2</v>
       </c>
       <c r="B38" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -3</v>
+        <v>dc.w 2</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
         <f t="shared" ca="1" si="1"/>
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="B39" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -3</v>
+        <v>dc.w -2</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -943,11 +943,11 @@
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="B41" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 2</v>
+        <v>dc.w -1</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -963,61 +963,61 @@
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43">
         <f t="shared" ca="1" si="1"/>
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="B43" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -2</v>
+        <v>dc.w -3</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44">
         <f t="shared" ca="1" si="1"/>
-        <v>-3</v>
+        <v>3</v>
       </c>
       <c r="B44" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -3</v>
+        <v>dc.w 3</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45">
         <f t="shared" ca="1" si="1"/>
-        <v>-3</v>
+        <v>1</v>
       </c>
       <c r="B45" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -3</v>
+        <v>dc.w 1</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="B46" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 2</v>
+        <v>dc.w -3</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47">
         <f t="shared" ca="1" si="1"/>
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="B47" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -1</v>
+        <v>dc.w 3</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="B48" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 2</v>
+        <v>dc.w -2</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -1033,11 +1033,11 @@
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="B50" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 1</v>
+        <v>dc.w -2</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -1063,71 +1063,71 @@
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53">
         <f t="shared" ca="1" si="1"/>
-        <v>-3</v>
+        <v>3</v>
       </c>
       <c r="B53" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -3</v>
+        <v>dc.w 3</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>-3</v>
       </c>
       <c r="B54" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 1</v>
+        <v>dc.w -3</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55">
         <f t="shared" ca="1" si="1"/>
-        <v>-2</v>
+        <v>1</v>
       </c>
       <c r="B55" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -2</v>
+        <v>dc.w 1</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56">
         <f t="shared" ca="1" si="1"/>
-        <v>-3</v>
+        <v>1</v>
       </c>
       <c r="B56" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -3</v>
+        <v>dc.w 1</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B57" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 1</v>
+        <v>dc.w -1</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B58" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 3</v>
+        <v>dc.w 1</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B59" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 3</v>
+        <v>dc.w 2</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -1143,21 +1143,21 @@
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="B61" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 2</v>
+        <v>dc.w -2</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B62" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 1</v>
+        <v>dc.w -1</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -1173,11 +1173,11 @@
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64">
         <f t="shared" ca="1" si="1"/>
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="B64" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -1</v>
+        <v>dc.w -3</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -1203,231 +1203,231 @@
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67">
         <f t="shared" ca="1" si="2"/>
-        <v>-3</v>
+        <v>2</v>
       </c>
       <c r="B67" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -3</v>
+        <v>dc.w 2</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68">
         <f t="shared" ca="1" si="2"/>
-        <v>-3</v>
+        <v>2</v>
       </c>
       <c r="B68" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -3</v>
+        <v>dc.w 2</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B69" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 1</v>
+        <v>dc.w 3</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B70" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 3</v>
+        <v>dc.w 2</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="B71" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 3</v>
+        <v>dc.w -1</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B72" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 3</v>
+        <v>dc.w 2</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73">
         <f t="shared" ca="1" si="2"/>
-        <v>-2</v>
+        <v>3</v>
       </c>
       <c r="B73" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -2</v>
+        <v>dc.w 3</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74">
         <f t="shared" ca="1" si="2"/>
-        <v>-2</v>
+        <v>1</v>
       </c>
       <c r="B74" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -2</v>
+        <v>dc.w 1</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75">
         <f t="shared" ca="1" si="2"/>
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="B75" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -2</v>
+        <v>dc.w -1</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76">
         <f t="shared" ca="1" si="2"/>
-        <v>-3</v>
+        <v>3</v>
       </c>
       <c r="B76" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -3</v>
+        <v>dc.w 3</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="B77" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 2</v>
+        <v>dc.w -3</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78">
         <f t="shared" ca="1" si="2"/>
-        <v>-3</v>
+        <v>1</v>
       </c>
       <c r="B78" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -3</v>
+        <v>dc.w 1</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79">
         <f t="shared" ca="1" si="2"/>
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="B79" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -3</v>
+        <v>dc.w -1</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>-3</v>
       </c>
       <c r="B80" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 3</v>
+        <v>dc.w -3</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>-2</v>
       </c>
       <c r="B81" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 3</v>
+        <v>dc.w -2</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>-2</v>
       </c>
       <c r="B82" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 3</v>
+        <v>dc.w -2</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83">
         <f t="shared" ca="1" si="2"/>
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="B83" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -1</v>
+        <v>dc.w -3</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84">
         <f t="shared" ca="1" si="2"/>
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="B84" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -1</v>
+        <v>dc.w -3</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85">
         <f t="shared" ca="1" si="2"/>
-        <v>-2</v>
+        <v>3</v>
       </c>
       <c r="B85" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -2</v>
+        <v>dc.w 3</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="B86" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 2</v>
+        <v>dc.w -1</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B87" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 2</v>
+        <v>dc.w 1</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="B88" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 2</v>
+        <v>dc.w -2</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B89" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 3</v>
+        <v>dc.w 2</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
@@ -1443,21 +1443,21 @@
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91">
         <f t="shared" ca="1" si="2"/>
-        <v>-3</v>
+        <v>1</v>
       </c>
       <c r="B91" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -3</v>
+        <v>dc.w 1</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>-3</v>
       </c>
       <c r="B92" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 1</v>
+        <v>dc.w -3</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
@@ -1473,21 +1473,21 @@
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="B94" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w 2</v>
+        <v>dc.w -1</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95">
         <f t="shared" ca="1" si="2"/>
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="B95" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -2</v>
+        <v>dc.w 2</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
@@ -1503,51 +1503,51 @@
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97">
         <f t="shared" ca="1" si="2"/>
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="B97" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -2</v>
+        <v>dc.w -3</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98">
         <f t="shared" ca="1" si="2"/>
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="B98" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -2</v>
+        <v>dc.w -1</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99">
         <f t="shared" ca="1" si="2"/>
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="B99" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -1</v>
+        <v>dc.w -3</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100">
         <f t="shared" ca="1" si="2"/>
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="B100" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -2</v>
+        <v>dc.w -3</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101">
         <f t="shared" ca="1" si="2"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B101" t="str">
         <f ca="1">"dc.w " &amp;Tabelle1[[#This Row],[Zufallszahl]]</f>
-        <v>dc.w -1</v>
+        <v>dc.w 1</v>
       </c>
     </row>
   </sheetData>
@@ -1560,10 +1560,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E59E07D8-3039-4DAB-963A-47C134361A80}">
-  <dimension ref="A1:B101"/>
+  <dimension ref="A1:B197"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="B101" sqref="B101"/>
+    <sheetView topLeftCell="A175" workbookViewId="0">
+      <selection activeCell="D195" sqref="D195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1581,29 +1581,29 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>-1</v>
+        <v>-7</v>
       </c>
       <c r="B2" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w -1</v>
+        <v>dc.w -7</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>-2</v>
+        <v>-6</v>
       </c>
       <c r="B3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w -2</v>
+        <v>dc.w -6</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>-3</v>
+        <v>-5</v>
       </c>
       <c r="B4" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w -3</v>
+        <v>dc.w -5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1617,146 +1617,146 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="B6" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w -5</v>
+        <v>dc.w -3</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="B7" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w 1</v>
+        <v>dc.w -2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="B8" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w 2</v>
+        <v>dc.w -1</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B9" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w 3</v>
+        <v>dc.w 1</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B10" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w 4</v>
+        <v>dc.w 2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B11" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w 5</v>
+        <v>dc.w 3</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="B12" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w -1</v>
+        <v>dc.w 4</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>-2</v>
+        <v>5</v>
       </c>
       <c r="B13" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w -2</v>
+        <v>dc.w 5</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>-3</v>
+        <v>6</v>
       </c>
       <c r="B14" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w -3</v>
+        <v>dc.w 6</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>-4</v>
+        <v>7</v>
       </c>
       <c r="B15" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w -4</v>
+        <v>dc.w 7</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>-5</v>
+        <v>-7</v>
       </c>
       <c r="B16" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w -5</v>
+        <v>dc.w -7</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>1</v>
+        <v>-6</v>
       </c>
       <c r="B17" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w 1</v>
+        <v>dc.w -6</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>2</v>
+        <v>-5</v>
       </c>
       <c r="B18" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w 2</v>
+        <v>dc.w -5</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>3</v>
+        <v>-4</v>
       </c>
       <c r="B19" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w 3</v>
+        <v>dc.w -4</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>4</v>
+        <v>-3</v>
       </c>
       <c r="B20" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w 4</v>
+        <v>dc.w -3</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>5</v>
+        <v>-2</v>
       </c>
       <c r="B21" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w 5</v>
+        <v>dc.w -2</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -1770,101 +1770,101 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>-2</v>
+        <v>1</v>
       </c>
       <c r="B23" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w -2</v>
+        <v>dc.w 1</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>-3</v>
+        <v>2</v>
       </c>
       <c r="B24" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w -3</v>
+        <v>dc.w 2</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>-4</v>
+        <v>3</v>
       </c>
       <c r="B25" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w -4</v>
+        <v>dc.w 3</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>-5</v>
+        <v>4</v>
       </c>
       <c r="B26" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w -5</v>
+        <v>dc.w 4</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B27" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w 1</v>
+        <v>dc.w 5</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B28" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w 2</v>
+        <v>dc.w 6</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B29" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w 3</v>
+        <v>dc.w 7</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>4</v>
+        <v>-7</v>
       </c>
       <c r="B30" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w 4</v>
+        <v>dc.w -7</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>5</v>
+        <v>-6</v>
       </c>
       <c r="B31" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w 5</v>
+        <v>dc.w -6</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>-1</v>
+        <v>-5</v>
       </c>
       <c r="B32" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w -1</v>
+        <v>dc.w -5</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>-2</v>
+        <v>-4</v>
       </c>
       <c r="B33" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w -2</v>
+        <v>dc.w -4</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -1878,20 +1878,20 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>-4</v>
+        <v>-2</v>
       </c>
       <c r="B35" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w -4</v>
+        <v>dc.w -2</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>-5</v>
+        <v>-1</v>
       </c>
       <c r="B36" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w -5</v>
+        <v>dc.w -1</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -1941,38 +1941,38 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="B42" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w -1</v>
+        <v>dc.w 6</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>-2</v>
+        <v>7</v>
       </c>
       <c r="B43" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w -2</v>
+        <v>dc.w 7</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>-3</v>
+        <v>-7</v>
       </c>
       <c r="B44" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w -3</v>
+        <v>dc.w -7</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>-4</v>
+        <v>-6</v>
       </c>
       <c r="B45" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w -4</v>
+        <v>dc.w -6</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -1986,146 +1986,146 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>1</v>
+        <v>-4</v>
       </c>
       <c r="B47" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w 1</v>
+        <v>dc.w -4</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="B48" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w 2</v>
+        <v>dc.w -3</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>3</v>
+        <v>-2</v>
       </c>
       <c r="B49" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w 3</v>
+        <v>dc.w -2</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>4</v>
+        <v>-1</v>
       </c>
       <c r="B50" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w 4</v>
+        <v>dc.w -1</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B51" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w 5</v>
+        <v>dc.w 1</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="B52" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w -1</v>
+        <v>dc.w 2</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>-2</v>
+        <v>3</v>
       </c>
       <c r="B53" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w -2</v>
+        <v>dc.w 3</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>-3</v>
+        <v>4</v>
       </c>
       <c r="B54" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w -3</v>
+        <v>dc.w 4</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>-4</v>
+        <v>5</v>
       </c>
       <c r="B55" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w -4</v>
+        <v>dc.w 5</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>-5</v>
+        <v>6</v>
       </c>
       <c r="B56" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w -5</v>
+        <v>dc.w 6</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B57" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w 1</v>
+        <v>dc.w 7</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>2</v>
+        <v>-7</v>
       </c>
       <c r="B58" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w 2</v>
+        <v>dc.w -7</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>3</v>
+        <v>-6</v>
       </c>
       <c r="B59" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w 3</v>
+        <v>dc.w -6</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>4</v>
+        <v>-5</v>
       </c>
       <c r="B60" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w 4</v>
+        <v>dc.w -5</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>5</v>
+        <v>-4</v>
       </c>
       <c r="B61" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w 5</v>
+        <v>dc.w -4</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="B62" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w -1</v>
+        <v>dc.w -3</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -2139,101 +2139,101 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="B64" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w -3</v>
+        <v>dc.w -1</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>-4</v>
+        <v>1</v>
       </c>
       <c r="B65" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w -4</v>
+        <v>dc.w 1</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>-5</v>
+        <v>2</v>
       </c>
       <c r="B66" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w -5</v>
+        <v>dc.w 2</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B67" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w 1</v>
+        <v>dc.w 3</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B68" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w 2</v>
+        <v>dc.w 4</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B69" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w 3</v>
+        <v>dc.w 5</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B70" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w 4</v>
+        <v>dc.w 6</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B71" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w 5</v>
+        <v>dc.w 7</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>-1</v>
+        <v>-7</v>
       </c>
       <c r="B72" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w -1</v>
+        <v>dc.w -7</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>-2</v>
+        <v>-6</v>
       </c>
       <c r="B73" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w -2</v>
+        <v>dc.w -6</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>-3</v>
+        <v>-5</v>
       </c>
       <c r="B74" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w -3</v>
+        <v>dc.w -5</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -2247,146 +2247,146 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="B76" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w -5</v>
+        <v>dc.w -3</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="B77" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w 1</v>
+        <v>dc.w -2</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="B78" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w 2</v>
+        <v>dc.w -1</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B79" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w 3</v>
+        <v>dc.w 1</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B80" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w 4</v>
+        <v>dc.w 2</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B81" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w 5</v>
+        <v>dc.w 3</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="B82" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w -1</v>
+        <v>dc.w 4</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>-2</v>
+        <v>5</v>
       </c>
       <c r="B83" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w -2</v>
+        <v>dc.w 5</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>-3</v>
+        <v>6</v>
       </c>
       <c r="B84" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w -3</v>
+        <v>dc.w 6</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>-4</v>
+        <v>7</v>
       </c>
       <c r="B85" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w -4</v>
+        <v>dc.w 7</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>-5</v>
+        <v>-7</v>
       </c>
       <c r="B86" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w -5</v>
+        <v>dc.w -7</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>1</v>
+        <v>-6</v>
       </c>
       <c r="B87" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w 1</v>
+        <v>dc.w -6</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>2</v>
+        <v>-5</v>
       </c>
       <c r="B88" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w 2</v>
+        <v>dc.w -5</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>3</v>
+        <v>-4</v>
       </c>
       <c r="B89" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w 3</v>
+        <v>dc.w -4</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>4</v>
+        <v>-3</v>
       </c>
       <c r="B90" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w 4</v>
+        <v>dc.w -3</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>5</v>
+        <v>-2</v>
       </c>
       <c r="B91" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w 5</v>
+        <v>dc.w -2</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
@@ -2400,83 +2400,947 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>-2</v>
+        <v>1</v>
       </c>
       <c r="B93" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w -2</v>
+        <v>dc.w 1</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>-3</v>
+        <v>2</v>
       </c>
       <c r="B94" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w -3</v>
+        <v>dc.w 2</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>-4</v>
+        <v>3</v>
       </c>
       <c r="B95" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w -4</v>
+        <v>dc.w 3</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>-5</v>
+        <v>4</v>
       </c>
       <c r="B96" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w -5</v>
+        <v>dc.w 4</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B97" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w 1</v>
+        <v>dc.w 5</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B98" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w 2</v>
+        <v>dc.w 6</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B99" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w 3</v>
+        <v>dc.w 7</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>4</v>
+        <v>-7</v>
       </c>
       <c r="B100" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
-        <v>dc.w 4</v>
+        <v>dc.w -7</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101">
+        <v>-6</v>
+      </c>
+      <c r="B101" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -6</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>-5</v>
+      </c>
+      <c r="B102" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -5</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>-4</v>
+      </c>
+      <c r="B103" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -4</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>-3</v>
+      </c>
+      <c r="B104" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>-2</v>
+      </c>
+      <c r="B105" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>-1</v>
+      </c>
+      <c r="B106" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>1</v>
+      </c>
+      <c r="B107" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>2</v>
+      </c>
+      <c r="B108" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>3</v>
+      </c>
+      <c r="B109" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 3</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>4</v>
+      </c>
+      <c r="B110" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 4</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111">
         <v>5</v>
       </c>
-      <c r="B101" s="3" t="str">
+      <c r="B111" s="3" t="str">
         <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
         <v>dc.w 5</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>6</v>
+      </c>
+      <c r="B112" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 6</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>7</v>
+      </c>
+      <c r="B113" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 7</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>-7</v>
+      </c>
+      <c r="B114" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -7</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>-6</v>
+      </c>
+      <c r="B115" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -6</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>-5</v>
+      </c>
+      <c r="B116" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -5</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>-4</v>
+      </c>
+      <c r="B117" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -4</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>-3</v>
+      </c>
+      <c r="B118" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -3</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>-2</v>
+      </c>
+      <c r="B119" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>-1</v>
+      </c>
+      <c r="B120" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>1</v>
+      </c>
+      <c r="B121" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>2</v>
+      </c>
+      <c r="B122" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 2</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>3</v>
+      </c>
+      <c r="B123" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 3</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>4</v>
+      </c>
+      <c r="B124" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 4</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>5</v>
+      </c>
+      <c r="B125" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 5</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>6</v>
+      </c>
+      <c r="B126" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 6</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>7</v>
+      </c>
+      <c r="B127" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 7</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>-7</v>
+      </c>
+      <c r="B128" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -7</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>-6</v>
+      </c>
+      <c r="B129" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -6</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>-5</v>
+      </c>
+      <c r="B130" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -5</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>-4</v>
+      </c>
+      <c r="B131" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -4</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>-3</v>
+      </c>
+      <c r="B132" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -3</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>-2</v>
+      </c>
+      <c r="B133" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -2</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>-1</v>
+      </c>
+      <c r="B134" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>1</v>
+      </c>
+      <c r="B135" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>2</v>
+      </c>
+      <c r="B136" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 2</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>3</v>
+      </c>
+      <c r="B137" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 3</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>4</v>
+      </c>
+      <c r="B138" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 4</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>5</v>
+      </c>
+      <c r="B139" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 5</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>6</v>
+      </c>
+      <c r="B140" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 6</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>7</v>
+      </c>
+      <c r="B141" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 7</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>-7</v>
+      </c>
+      <c r="B142" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -7</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>-6</v>
+      </c>
+      <c r="B143" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -6</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>-5</v>
+      </c>
+      <c r="B144" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -5</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>-4</v>
+      </c>
+      <c r="B145" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -4</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>-3</v>
+      </c>
+      <c r="B146" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -3</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>-2</v>
+      </c>
+      <c r="B147" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -2</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>-1</v>
+      </c>
+      <c r="B148" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>1</v>
+      </c>
+      <c r="B149" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>2</v>
+      </c>
+      <c r="B150" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 2</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>3</v>
+      </c>
+      <c r="B151" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 3</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>4</v>
+      </c>
+      <c r="B152" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 4</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>5</v>
+      </c>
+      <c r="B153" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 5</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>6</v>
+      </c>
+      <c r="B154" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 6</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>7</v>
+      </c>
+      <c r="B155" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 7</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>-7</v>
+      </c>
+      <c r="B156" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -7</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>-6</v>
+      </c>
+      <c r="B157" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -6</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>-5</v>
+      </c>
+      <c r="B158" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -5</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>-4</v>
+      </c>
+      <c r="B159" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -4</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>-3</v>
+      </c>
+      <c r="B160" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -3</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>-2</v>
+      </c>
+      <c r="B161" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -2</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <v>-1</v>
+      </c>
+      <c r="B162" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <v>1</v>
+      </c>
+      <c r="B163" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>2</v>
+      </c>
+      <c r="B164" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 2</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A165">
+        <v>3</v>
+      </c>
+      <c r="B165" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 3</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A166">
+        <v>4</v>
+      </c>
+      <c r="B166" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 4</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <v>5</v>
+      </c>
+      <c r="B167" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 5</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A168">
+        <v>6</v>
+      </c>
+      <c r="B168" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 6</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A169">
+        <v>7</v>
+      </c>
+      <c r="B169" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 7</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <v>-7</v>
+      </c>
+      <c r="B170" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -7</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <v>-6</v>
+      </c>
+      <c r="B171" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -6</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <v>-5</v>
+      </c>
+      <c r="B172" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -5</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <v>-4</v>
+      </c>
+      <c r="B173" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -4</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>-3</v>
+      </c>
+      <c r="B174" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -3</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <v>-2</v>
+      </c>
+      <c r="B175" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -2</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>-1</v>
+      </c>
+      <c r="B176" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -1</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <v>1</v>
+      </c>
+      <c r="B177" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 1</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <v>2</v>
+      </c>
+      <c r="B178" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 2</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A179">
+        <v>3</v>
+      </c>
+      <c r="B179" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 3</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A180">
+        <v>4</v>
+      </c>
+      <c r="B180" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 4</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A181">
+        <v>5</v>
+      </c>
+      <c r="B181" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 5</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A182">
+        <v>6</v>
+      </c>
+      <c r="B182" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 6</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <v>7</v>
+      </c>
+      <c r="B183" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 7</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <v>-7</v>
+      </c>
+      <c r="B184" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -7</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A185">
+        <v>-6</v>
+      </c>
+      <c r="B185" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -6</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A186">
+        <v>-5</v>
+      </c>
+      <c r="B186" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -5</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A187">
+        <v>-4</v>
+      </c>
+      <c r="B187" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -4</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A188">
+        <v>-3</v>
+      </c>
+      <c r="B188" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -3</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A189">
+        <v>-2</v>
+      </c>
+      <c r="B189" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -2</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A190">
+        <v>-1</v>
+      </c>
+      <c r="B190" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w -1</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A191">
+        <v>1</v>
+      </c>
+      <c r="B191" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 1</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A192">
+        <v>2</v>
+      </c>
+      <c r="B192" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 2</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A193">
+        <v>3</v>
+      </c>
+      <c r="B193" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 3</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A194">
+        <v>4</v>
+      </c>
+      <c r="B194" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 4</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A195">
+        <v>5</v>
+      </c>
+      <c r="B195" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 5</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A196">
+        <v>6</v>
+      </c>
+      <c r="B196" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 6</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A197">
+        <v>7</v>
+      </c>
+      <c r="B197" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle2[[#This Row],[Zahl]]</f>
+        <v>dc.w 7</v>
       </c>
     </row>
   </sheetData>
@@ -2489,10 +3353,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C888866-0535-4EEA-B92A-DFAC3598319B}">
-  <dimension ref="A1:B104"/>
+  <dimension ref="A1:B197"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="B105" sqref="B105"/>
+    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
+      <selection activeCell="G194" sqref="G194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2510,912 +3374,1767 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>-5</v>
+        <v>-7</v>
       </c>
       <c r="B2" s="2" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w -5</v>
+        <v>dc.w -7</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>-5</v>
+        <v>-7</v>
       </c>
       <c r="B3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w -5</v>
+        <v>dc.w -7</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>-5</v>
+        <v>-7</v>
       </c>
       <c r="B4" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w -5</v>
+        <v>dc.w -7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>-5</v>
+        <v>-7</v>
       </c>
       <c r="B5" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w -5</v>
+        <v>dc.w -7</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>-5</v>
+        <v>-7</v>
       </c>
       <c r="B6" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w -5</v>
+        <v>dc.w -7</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>-5</v>
+        <v>-7</v>
       </c>
       <c r="B7" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w -5</v>
+        <v>dc.w -7</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>-5</v>
+        <v>-7</v>
       </c>
       <c r="B8" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w -5</v>
+        <v>dc.w -7</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>-5</v>
+        <v>-7</v>
       </c>
       <c r="B9" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w -5</v>
+        <v>dc.w -7</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>-5</v>
+        <v>-7</v>
       </c>
       <c r="B10" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w -5</v>
+        <v>dc.w -7</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>-5</v>
+        <v>-7</v>
       </c>
       <c r="B11" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w -5</v>
+        <v>dc.w -7</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>-4</v>
+        <v>-7</v>
       </c>
       <c r="B12" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w -4</v>
+        <v>dc.w -7</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>-4</v>
+        <v>-7</v>
       </c>
       <c r="B13" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w -4</v>
+        <v>dc.w -7</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>-4</v>
+        <v>-7</v>
       </c>
       <c r="B14" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w -4</v>
+        <v>dc.w -7</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>-4</v>
+        <v>-7</v>
       </c>
       <c r="B15" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w -4</v>
+        <v>dc.w -7</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>-4</v>
+        <v>-6</v>
       </c>
       <c r="B16" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w -4</v>
+        <v>dc.w -6</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>-4</v>
+        <v>-6</v>
       </c>
       <c r="B17" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w -4</v>
+        <v>dc.w -6</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>-4</v>
+        <v>-6</v>
       </c>
       <c r="B18" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w -4</v>
+        <v>dc.w -6</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>-4</v>
+        <v>-6</v>
       </c>
       <c r="B19" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w -4</v>
+        <v>dc.w -6</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>-4</v>
+        <v>-6</v>
       </c>
       <c r="B20" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w -4</v>
+        <v>dc.w -6</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>-4</v>
+        <v>-6</v>
       </c>
       <c r="B21" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w -4</v>
+        <v>dc.w -6</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>-3</v>
+        <v>-6</v>
       </c>
       <c r="B22" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w -3</v>
+        <v>dc.w -6</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>-3</v>
+        <v>-6</v>
       </c>
       <c r="B23" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w -3</v>
+        <v>dc.w -6</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>-3</v>
+        <v>-6</v>
       </c>
       <c r="B24" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w -3</v>
+        <v>dc.w -6</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>-3</v>
+        <v>-6</v>
       </c>
       <c r="B25" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w -3</v>
+        <v>dc.w -6</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>-3</v>
+        <v>-6</v>
       </c>
       <c r="B26" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w -3</v>
+        <v>dc.w -6</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>-3</v>
+        <v>-6</v>
       </c>
       <c r="B27" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w -3</v>
+        <v>dc.w -6</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>-3</v>
+        <v>-6</v>
       </c>
       <c r="B28" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w -3</v>
+        <v>dc.w -6</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>-3</v>
+        <v>-6</v>
       </c>
       <c r="B29" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w -3</v>
+        <v>dc.w -6</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>-3</v>
+        <v>-5</v>
       </c>
       <c r="B30" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w -3</v>
+        <v>dc.w -5</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>-3</v>
+        <v>-5</v>
       </c>
       <c r="B31" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w -3</v>
+        <v>dc.w -5</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>-2</v>
+        <v>-5</v>
       </c>
       <c r="B32" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w -2</v>
+        <v>dc.w -5</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>-2</v>
+        <v>-5</v>
       </c>
       <c r="B33" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w -2</v>
+        <v>dc.w -5</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>-2</v>
+        <v>-5</v>
       </c>
       <c r="B34" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w -2</v>
+        <v>dc.w -5</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>-2</v>
+        <v>-5</v>
       </c>
       <c r="B35" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w -2</v>
+        <v>dc.w -5</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>-2</v>
+        <v>-5</v>
       </c>
       <c r="B36" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w -2</v>
+        <v>dc.w -5</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>-2</v>
+        <v>-5</v>
       </c>
       <c r="B37" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w -2</v>
+        <v>dc.w -5</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>-2</v>
+        <v>-5</v>
       </c>
       <c r="B38" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w -2</v>
+        <v>dc.w -5</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>-2</v>
+        <v>-5</v>
       </c>
       <c r="B39" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w -2</v>
+        <v>dc.w -5</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>-2</v>
+        <v>-5</v>
       </c>
       <c r="B40" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w -2</v>
+        <v>dc.w -5</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>-2</v>
+        <v>-5</v>
       </c>
       <c r="B41" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w -2</v>
+        <v>dc.w -5</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>-1</v>
+        <v>-5</v>
       </c>
       <c r="B42" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w -1</v>
+        <v>dc.w -5</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>-1</v>
+        <v>-5</v>
       </c>
       <c r="B43" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w -1</v>
+        <v>dc.w -5</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>-1</v>
+        <v>-4</v>
       </c>
       <c r="B44" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w -1</v>
+        <v>dc.w -4</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>-1</v>
+        <v>-4</v>
       </c>
       <c r="B45" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w -1</v>
+        <v>dc.w -4</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>-1</v>
+        <v>-4</v>
       </c>
       <c r="B46" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w -1</v>
+        <v>dc.w -4</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>-1</v>
+        <v>-4</v>
       </c>
       <c r="B47" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w -1</v>
+        <v>dc.w -4</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>-1</v>
+        <v>-4</v>
       </c>
       <c r="B48" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w -1</v>
+        <v>dc.w -4</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>-1</v>
+        <v>-4</v>
       </c>
       <c r="B49" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w -1</v>
+        <v>dc.w -4</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>-1</v>
+        <v>-4</v>
       </c>
       <c r="B50" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w -1</v>
+        <v>dc.w -4</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>-1</v>
+        <v>-4</v>
       </c>
       <c r="B51" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w -1</v>
+        <v>dc.w -4</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>1</v>
+        <v>-4</v>
       </c>
       <c r="B52" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w 1</v>
+        <v>dc.w -4</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>1</v>
+        <v>-4</v>
       </c>
       <c r="B53" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w 1</v>
+        <v>dc.w -4</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>1</v>
+        <v>-4</v>
       </c>
       <c r="B54" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w 1</v>
+        <v>dc.w -4</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>1</v>
+        <v>-4</v>
       </c>
       <c r="B55" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w 1</v>
+        <v>dc.w -4</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>1</v>
+        <v>-4</v>
       </c>
       <c r="B56" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w 1</v>
+        <v>dc.w -4</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>1</v>
+        <v>-4</v>
       </c>
       <c r="B57" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w 1</v>
+        <v>dc.w -4</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>1</v>
+        <v>-3</v>
       </c>
       <c r="B58" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w 1</v>
+        <v>dc.w -3</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>1</v>
+        <v>-3</v>
       </c>
       <c r="B59" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w 1</v>
+        <v>dc.w -3</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>1</v>
+        <v>-3</v>
       </c>
       <c r="B60" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w 1</v>
+        <v>dc.w -3</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>1</v>
+        <v>-3</v>
       </c>
       <c r="B61" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w 1</v>
+        <v>dc.w -3</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="B62" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w 2</v>
+        <v>dc.w -3</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="B63" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w 2</v>
+        <v>dc.w -3</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="B64" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w 2</v>
+        <v>dc.w -3</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="B65" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w 2</v>
+        <v>dc.w -3</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="B66" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w 2</v>
+        <v>dc.w -3</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="B67" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w 2</v>
+        <v>dc.w -3</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="B68" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w 2</v>
+        <v>dc.w -3</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="B69" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w 2</v>
+        <v>dc.w -3</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="B70" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w 2</v>
+        <v>dc.w -3</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="B71" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w 2</v>
+        <v>dc.w -3</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>3</v>
+        <v>-2</v>
       </c>
       <c r="B72" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w 3</v>
+        <v>dc.w -2</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>3</v>
+        <v>-2</v>
       </c>
       <c r="B73" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w 3</v>
+        <v>dc.w -2</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>3</v>
+        <v>-2</v>
       </c>
       <c r="B74" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w 3</v>
+        <v>dc.w -2</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>3</v>
+        <v>-2</v>
       </c>
       <c r="B75" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w 3</v>
+        <v>dc.w -2</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>3</v>
+        <v>-2</v>
       </c>
       <c r="B76" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w 3</v>
+        <v>dc.w -2</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>3</v>
+        <v>-2</v>
       </c>
       <c r="B77" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w 3</v>
+        <v>dc.w -2</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>3</v>
+        <v>-2</v>
       </c>
       <c r="B78" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w 3</v>
+        <v>dc.w -2</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>3</v>
+        <v>-2</v>
       </c>
       <c r="B79" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w 3</v>
+        <v>dc.w -2</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>3</v>
+        <v>-2</v>
       </c>
       <c r="B80" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w 3</v>
+        <v>dc.w -2</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>3</v>
+        <v>-2</v>
       </c>
       <c r="B81" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w 3</v>
+        <v>dc.w -2</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>4</v>
+        <v>-2</v>
       </c>
       <c r="B82" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w 4</v>
+        <v>dc.w -2</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>4</v>
+        <v>-2</v>
       </c>
       <c r="B83" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w 4</v>
+        <v>dc.w -2</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>4</v>
+        <v>-2</v>
       </c>
       <c r="B84" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w 4</v>
+        <v>dc.w -2</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>4</v>
+        <v>-2</v>
       </c>
       <c r="B85" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w 4</v>
+        <v>dc.w -2</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>4</v>
+        <v>-1</v>
       </c>
       <c r="B86" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w 4</v>
+        <v>dc.w -1</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>4</v>
+        <v>-1</v>
       </c>
       <c r="B87" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w 4</v>
+        <v>dc.w -1</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>4</v>
+        <v>-1</v>
       </c>
       <c r="B88" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w 4</v>
+        <v>dc.w -1</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>4</v>
+        <v>-1</v>
       </c>
       <c r="B89" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w 4</v>
+        <v>dc.w -1</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>4</v>
+        <v>-1</v>
       </c>
       <c r="B90" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w 4</v>
+        <v>dc.w -1</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>4</v>
+        <v>-1</v>
       </c>
       <c r="B91" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w 4</v>
+        <v>dc.w -1</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>5</v>
+        <v>-1</v>
       </c>
       <c r="B92" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w 5</v>
+        <v>dc.w -1</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>5</v>
+        <v>-1</v>
       </c>
       <c r="B93" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w 5</v>
+        <v>dc.w -1</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>5</v>
+        <v>-1</v>
       </c>
       <c r="B94" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w 5</v>
+        <v>dc.w -1</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>5</v>
+        <v>-1</v>
       </c>
       <c r="B95" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w 5</v>
+        <v>dc.w -1</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>5</v>
+        <v>-1</v>
       </c>
       <c r="B96" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w 5</v>
+        <v>dc.w -1</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>5</v>
+        <v>-1</v>
       </c>
       <c r="B97" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w 5</v>
+        <v>dc.w -1</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>5</v>
+        <v>-1</v>
       </c>
       <c r="B98" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w 5</v>
+        <v>dc.w -1</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>5</v>
+        <v>-1</v>
       </c>
       <c r="B99" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w 5</v>
+        <v>dc.w -1</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B100" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
-        <v>dc.w 5</v>
+        <v>dc.w 1</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101">
+        <v>1</v>
+      </c>
+      <c r="B101" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>1</v>
+      </c>
+      <c r="B102" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>1</v>
+      </c>
+      <c r="B103" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>1</v>
+      </c>
+      <c r="B104" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>1</v>
+      </c>
+      <c r="B105" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>1</v>
+      </c>
+      <c r="B106" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>1</v>
+      </c>
+      <c r="B107" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>1</v>
+      </c>
+      <c r="B108" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>1</v>
+      </c>
+      <c r="B109" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>1</v>
+      </c>
+      <c r="B110" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>1</v>
+      </c>
+      <c r="B111" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>1</v>
+      </c>
+      <c r="B112" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>1</v>
+      </c>
+      <c r="B113" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>2</v>
+      </c>
+      <c r="B114" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 2</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>2</v>
+      </c>
+      <c r="B115" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>2</v>
+      </c>
+      <c r="B116" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>2</v>
+      </c>
+      <c r="B117" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>2</v>
+      </c>
+      <c r="B118" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>2</v>
+      </c>
+      <c r="B119" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>2</v>
+      </c>
+      <c r="B120" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>2</v>
+      </c>
+      <c r="B121" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>2</v>
+      </c>
+      <c r="B122" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 2</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>2</v>
+      </c>
+      <c r="B123" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>2</v>
+      </c>
+      <c r="B124" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>2</v>
+      </c>
+      <c r="B125" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>2</v>
+      </c>
+      <c r="B126" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 2</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>2</v>
+      </c>
+      <c r="B127" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>3</v>
+      </c>
+      <c r="B128" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 3</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>3</v>
+      </c>
+      <c r="B129" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 3</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>3</v>
+      </c>
+      <c r="B130" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 3</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>3</v>
+      </c>
+      <c r="B131" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 3</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>3</v>
+      </c>
+      <c r="B132" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 3</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>3</v>
+      </c>
+      <c r="B133" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 3</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>3</v>
+      </c>
+      <c r="B134" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 3</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>3</v>
+      </c>
+      <c r="B135" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 3</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>3</v>
+      </c>
+      <c r="B136" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 3</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>3</v>
+      </c>
+      <c r="B137" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 3</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>3</v>
+      </c>
+      <c r="B138" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 3</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>3</v>
+      </c>
+      <c r="B139" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 3</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>3</v>
+      </c>
+      <c r="B140" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 3</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>3</v>
+      </c>
+      <c r="B141" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 3</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>4</v>
+      </c>
+      <c r="B142" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 4</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>4</v>
+      </c>
+      <c r="B143" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 4</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>4</v>
+      </c>
+      <c r="B144" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 4</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>4</v>
+      </c>
+      <c r="B145" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 4</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>4</v>
+      </c>
+      <c r="B146" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 4</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>4</v>
+      </c>
+      <c r="B147" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 4</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>4</v>
+      </c>
+      <c r="B148" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 4</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>4</v>
+      </c>
+      <c r="B149" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 4</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>4</v>
+      </c>
+      <c r="B150" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 4</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>4</v>
+      </c>
+      <c r="B151" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 4</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>4</v>
+      </c>
+      <c r="B152" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 4</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>4</v>
+      </c>
+      <c r="B153" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 4</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>4</v>
+      </c>
+      <c r="B154" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 4</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>4</v>
+      </c>
+      <c r="B155" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 4</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156">
         <v>5</v>
       </c>
-      <c r="B101" s="3" t="str">
+      <c r="B156" s="3" t="str">
         <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
         <v>dc.w 5</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B102" s="3"/>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B103" s="3"/>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B104" s="3"/>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>5</v>
+      </c>
+      <c r="B157" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 5</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>5</v>
+      </c>
+      <c r="B158" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 5</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>5</v>
+      </c>
+      <c r="B159" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 5</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>5</v>
+      </c>
+      <c r="B160" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 5</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>5</v>
+      </c>
+      <c r="B161" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 5</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <v>5</v>
+      </c>
+      <c r="B162" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 5</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <v>5</v>
+      </c>
+      <c r="B163" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 5</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>5</v>
+      </c>
+      <c r="B164" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 5</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A165">
+        <v>5</v>
+      </c>
+      <c r="B165" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 5</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A166">
+        <v>5</v>
+      </c>
+      <c r="B166" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 5</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <v>5</v>
+      </c>
+      <c r="B167" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 5</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A168">
+        <v>5</v>
+      </c>
+      <c r="B168" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 5</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A169">
+        <v>5</v>
+      </c>
+      <c r="B169" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 5</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <v>6</v>
+      </c>
+      <c r="B170" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 6</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <v>6</v>
+      </c>
+      <c r="B171" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 6</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <v>6</v>
+      </c>
+      <c r="B172" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 6</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <v>6</v>
+      </c>
+      <c r="B173" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 6</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>6</v>
+      </c>
+      <c r="B174" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 6</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <v>6</v>
+      </c>
+      <c r="B175" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 6</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>6</v>
+      </c>
+      <c r="B176" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 6</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <v>6</v>
+      </c>
+      <c r="B177" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 6</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <v>6</v>
+      </c>
+      <c r="B178" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 6</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A179">
+        <v>6</v>
+      </c>
+      <c r="B179" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 6</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A180">
+        <v>6</v>
+      </c>
+      <c r="B180" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 6</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A181">
+        <v>6</v>
+      </c>
+      <c r="B181" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 6</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A182">
+        <v>6</v>
+      </c>
+      <c r="B182" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 6</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <v>6</v>
+      </c>
+      <c r="B183" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 6</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <v>7</v>
+      </c>
+      <c r="B184" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 7</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A185">
+        <v>7</v>
+      </c>
+      <c r="B185" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 7</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A186">
+        <v>7</v>
+      </c>
+      <c r="B186" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 7</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A187">
+        <v>7</v>
+      </c>
+      <c r="B187" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 7</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A188">
+        <v>7</v>
+      </c>
+      <c r="B188" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 7</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A189">
+        <v>7</v>
+      </c>
+      <c r="B189" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 7</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A190">
+        <v>7</v>
+      </c>
+      <c r="B190" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 7</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A191">
+        <v>7</v>
+      </c>
+      <c r="B191" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 7</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A192">
+        <v>7</v>
+      </c>
+      <c r="B192" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 7</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A193">
+        <v>7</v>
+      </c>
+      <c r="B193" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 7</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A194">
+        <v>7</v>
+      </c>
+      <c r="B194" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 7</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A195">
+        <v>7</v>
+      </c>
+      <c r="B195" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 7</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A196">
+        <v>7</v>
+      </c>
+      <c r="B196" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 7</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A197">
+        <v>7</v>
+      </c>
+      <c r="B197" s="3" t="str">
+        <f>"dc.w " &amp;Tabelle3[[#This Row],[Zahl]]</f>
+        <v>dc.w 7</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>